<commit_message>
Datum hinzugefügt, jetzt genauer
</commit_message>
<xml_diff>
--- a/Plan Facharbeit.xlsx
+++ b/Plan Facharbeit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenetusche/Desktop/Facharbeit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CC1148-FCB7-8448-B65C-892FDC1FB5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873E3AC3-BD59-DC4F-AAAC-46BC5503537B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7BDE49E7-83ED-EC42-A8B5-47A6A9BF310E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{7BDE49E7-83ED-EC42-A8B5-47A6A9BF310E}"/>
   </bookViews>
   <sheets>
     <sheet name="Allgemeiner Kalender" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="24">
   <si>
     <t>Aufgaben</t>
   </si>
@@ -163,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +239,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF833C0B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -633,12 +639,31 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF833C0B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -949,7 +974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1DCA6C-01EA-5242-8B8C-B662E9E2A75B}">
   <dimension ref="A2:U34"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1747,10 +1772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E6C06B-736E-4148-BC18-BFA92AB47EBF}">
-  <dimension ref="A1:AF26"/>
+  <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1905,126 +1930,186 @@
       </c>
     </row>
     <row r="3" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="74">
+        <v>1</v>
+      </c>
+      <c r="C3" s="74">
+        <v>2</v>
+      </c>
+      <c r="D3" s="74">
+        <v>3</v>
+      </c>
+      <c r="E3" s="74">
+        <v>4</v>
+      </c>
+      <c r="F3" s="74">
+        <v>5</v>
+      </c>
+      <c r="G3" s="74">
+        <v>6</v>
+      </c>
+      <c r="H3" s="74">
+        <v>7</v>
+      </c>
+      <c r="I3" s="74">
+        <v>8</v>
+      </c>
+      <c r="J3" s="74">
+        <v>9</v>
+      </c>
+      <c r="K3" s="74">
+        <v>10</v>
+      </c>
+      <c r="L3" s="74">
+        <v>11</v>
+      </c>
+      <c r="M3" s="74">
+        <v>12</v>
+      </c>
+      <c r="N3" s="74">
+        <v>13</v>
+      </c>
+      <c r="O3" s="74">
+        <v>14</v>
+      </c>
+      <c r="P3" s="75">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="74">
+        <v>16</v>
+      </c>
+      <c r="R3" s="75">
+        <v>17</v>
+      </c>
+      <c r="S3" s="74">
+        <v>18</v>
+      </c>
+      <c r="T3" s="75">
+        <v>19</v>
+      </c>
+      <c r="U3" s="74">
+        <v>20</v>
+      </c>
+      <c r="V3" s="75">
+        <v>21</v>
+      </c>
+      <c r="W3" s="74">
+        <v>22</v>
+      </c>
+      <c r="X3" s="75">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="74">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="74">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="74">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="74">
+        <v>27</v>
+      </c>
+      <c r="AC3" s="74">
+        <v>28</v>
+      </c>
+      <c r="AD3" s="74">
+        <v>29</v>
+      </c>
+      <c r="AE3" s="74">
+        <v>30</v>
+      </c>
+      <c r="AF3" s="74">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="12" t="s">
+      <c r="B4" s="42"/>
+      <c r="C4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12" t="s">
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="46" t="s">
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="46"/>
-      <c r="AA3" s="46"/>
-      <c r="AB3" s="46"/>
-      <c r="AC3" s="46"/>
-      <c r="AD3" s="46"/>
-      <c r="AE3" s="46" t="s">
+      <c r="Y4" s="46"/>
+      <c r="Z4" s="46"/>
+      <c r="AA4" s="46"/>
+      <c r="AB4" s="46"/>
+      <c r="AC4" s="46"/>
+      <c r="AD4" s="46"/>
+      <c r="AE4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="AF3" s="46"/>
-    </row>
-    <row r="4" spans="1:32" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="66" t="s">
+      <c r="AF4" s="46"/>
+    </row>
+    <row r="5" spans="1:32" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="48"/>
-      <c r="Y4" s="49"/>
-      <c r="Z4" s="49"/>
-      <c r="AA4" s="49"/>
-      <c r="AB4" s="49"/>
-      <c r="AC4" s="49"/>
-      <c r="AD4" s="53"/>
-      <c r="AE4" s="48"/>
-      <c r="AF4" s="53"/>
-    </row>
-    <row r="5" spans="1:32" ht="26" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="30"/>
+      <c r="X5" s="48"/>
+      <c r="Y5" s="49"/>
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="49"/>
+      <c r="AB5" s="49"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="53"/>
+      <c r="AE5" s="48"/>
+      <c r="AF5" s="53"/>
+    </row>
+    <row r="6" spans="1:32" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="36" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="50"/>
-      <c r="Y5" s="47"/>
-      <c r="Z5" s="47"/>
-      <c r="AA5" s="47"/>
-      <c r="AB5" s="47"/>
-      <c r="AC5" s="47"/>
-      <c r="AD5" s="54"/>
-      <c r="AE5" s="50"/>
-      <c r="AF5" s="54"/>
-    </row>
-    <row r="6" spans="1:32" ht="26" x14ac:dyDescent="0.3">
-      <c r="A6" s="61" t="s">
-        <v>9</v>
       </c>
       <c r="B6" s="27"/>
       <c r="C6" s="10"/>
@@ -2032,22 +2117,22 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="62"/>
-      <c r="S6" s="62"/>
-      <c r="T6" s="62"/>
-      <c r="U6" s="62"/>
-      <c r="V6" s="62"/>
-      <c r="W6" s="62"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="60"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="18"/>
       <c r="X6" s="50"/>
       <c r="Y6" s="47"/>
       <c r="Z6" s="47"/>
@@ -2059,8 +2144,8 @@
       <c r="AF6" s="54"/>
     </row>
     <row r="7" spans="1:32" ht="26" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
-        <v>22</v>
+      <c r="A7" s="61" t="s">
+        <v>9</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="10"/>
@@ -2068,35 +2153,35 @@
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="17"/>
-      <c r="AA7" s="17"/>
-      <c r="AB7" s="17"/>
-      <c r="AC7" s="47"/>
-      <c r="AD7" s="54"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="62"/>
+      <c r="T7" s="62"/>
+      <c r="U7" s="62"/>
+      <c r="V7" s="62"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="62"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="62"/>
+      <c r="AA7" s="62"/>
+      <c r="AB7" s="62"/>
+      <c r="AC7" s="62"/>
+      <c r="AD7" s="62"/>
       <c r="AE7" s="50"/>
       <c r="AF7" s="54"/>
     </row>
     <row r="8" spans="1:32" ht="26" x14ac:dyDescent="0.3">
-      <c r="A8" s="63" t="s">
-        <v>23</v>
+      <c r="A8" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="B8" s="27"/>
       <c r="C8" s="10"/>
@@ -2118,20 +2203,22 @@
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
-      <c r="V8" s="63"/>
-      <c r="W8" s="63"/>
-      <c r="X8" s="63"/>
-      <c r="Y8" s="63"/>
-      <c r="Z8" s="63"/>
-      <c r="AA8" s="63"/>
-      <c r="AB8" s="63"/>
-      <c r="AC8" s="63"/>
-      <c r="AD8" s="63"/>
-      <c r="AE8" s="63"/>
-      <c r="AF8" s="63"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="50"/>
+      <c r="AF8" s="54"/>
     </row>
     <row r="9" spans="1:32" ht="26" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
+      <c r="A9" s="63" t="s">
+        <v>23</v>
+      </c>
       <c r="B9" s="27"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -2152,17 +2239,17 @@
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="50"/>
-      <c r="Y9" s="47"/>
-      <c r="Z9" s="47"/>
-      <c r="AA9" s="47"/>
-      <c r="AB9" s="47"/>
-      <c r="AC9" s="47"/>
-      <c r="AD9" s="54"/>
-      <c r="AE9" s="50"/>
-      <c r="AF9" s="54"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="63"/>
+      <c r="X9" s="63"/>
+      <c r="Y9" s="63"/>
+      <c r="Z9" s="63"/>
+      <c r="AA9" s="63"/>
+      <c r="AB9" s="63"/>
+      <c r="AC9" s="63"/>
+      <c r="AD9" s="63"/>
+      <c r="AE9" s="63"/>
+      <c r="AF9" s="63"/>
     </row>
     <row r="10" spans="1:32" ht="26" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
@@ -2708,39 +2795,73 @@
       <c r="AE25" s="50"/>
       <c r="AF25" s="54"/>
     </row>
-    <row r="26" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-      <c r="T26" s="22"/>
-      <c r="U26" s="22"/>
-      <c r="V26" s="22"/>
-      <c r="W26" s="23"/>
-      <c r="X26" s="51"/>
-      <c r="Y26" s="52"/>
-      <c r="Z26" s="52"/>
-      <c r="AA26" s="52"/>
-      <c r="AB26" s="52"/>
-      <c r="AC26" s="52"/>
-      <c r="AD26" s="55"/>
-      <c r="AE26" s="51"/>
-      <c r="AF26" s="55"/>
+    <row r="26" spans="1:32" ht="26" x14ac:dyDescent="0.3">
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="18"/>
+      <c r="X26" s="50"/>
+      <c r="Y26" s="47"/>
+      <c r="Z26" s="47"/>
+      <c r="AA26" s="47"/>
+      <c r="AB26" s="47"/>
+      <c r="AC26" s="47"/>
+      <c r="AD26" s="54"/>
+      <c r="AE26" s="50"/>
+      <c r="AF26" s="54"/>
+    </row>
+    <row r="27" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="28"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="22"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="23"/>
+      <c r="X27" s="51"/>
+      <c r="Y27" s="52"/>
+      <c r="Z27" s="52"/>
+      <c r="AA27" s="52"/>
+      <c r="AB27" s="52"/>
+      <c r="AC27" s="52"/>
+      <c r="AD27" s="55"/>
+      <c r="AE27" s="51"/>
+      <c r="AF27" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2749,10 +2870,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7CB675A-1926-F04B-8B92-D8B33DD41347}">
-  <dimension ref="A1:AE27"/>
+  <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2840,7 +2961,7 @@
       <c r="AD2" s="43"/>
       <c r="AE2" s="43"/>
     </row>
-    <row r="3" spans="1:31" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>14</v>
       </c>
@@ -2936,115 +3057,175 @@
       </c>
     </row>
     <row r="4" spans="1:31" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="79">
+        <v>1</v>
+      </c>
+      <c r="C4" s="79">
+        <v>2</v>
+      </c>
+      <c r="D4" s="79">
+        <v>3</v>
+      </c>
+      <c r="E4" s="79">
+        <v>4</v>
+      </c>
+      <c r="F4" s="79">
+        <v>5</v>
+      </c>
+      <c r="G4" s="79">
+        <v>6</v>
+      </c>
+      <c r="H4" s="79">
+        <v>7</v>
+      </c>
+      <c r="I4" s="79">
+        <v>8</v>
+      </c>
+      <c r="J4" s="79">
+        <v>9</v>
+      </c>
+      <c r="K4" s="79">
+        <v>10</v>
+      </c>
+      <c r="L4" s="79">
+        <v>11</v>
+      </c>
+      <c r="M4" s="79">
+        <v>12</v>
+      </c>
+      <c r="N4" s="79">
+        <v>13</v>
+      </c>
+      <c r="O4" s="79">
+        <v>14</v>
+      </c>
+      <c r="P4" s="79">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="79">
+        <v>16</v>
+      </c>
+      <c r="R4" s="79">
+        <v>17</v>
+      </c>
+      <c r="S4" s="79">
+        <v>18</v>
+      </c>
+      <c r="T4" s="79">
+        <v>19</v>
+      </c>
+      <c r="U4" s="79">
+        <v>20</v>
+      </c>
+      <c r="V4" s="79">
+        <v>21</v>
+      </c>
+      <c r="W4" s="79">
+        <v>22</v>
+      </c>
+      <c r="X4" s="79">
+        <v>23</v>
+      </c>
+      <c r="Y4" s="79">
+        <v>24</v>
+      </c>
+      <c r="Z4" s="79">
+        <v>25</v>
+      </c>
+      <c r="AA4" s="79">
+        <v>26</v>
+      </c>
+      <c r="AB4" s="79">
+        <v>27</v>
+      </c>
+      <c r="AC4" s="79">
+        <v>28</v>
+      </c>
+      <c r="AD4" s="79">
+        <v>29</v>
+      </c>
+      <c r="AE4" s="79">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12" t="s">
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12" t="s">
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="46" t="s">
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="77"/>
+      <c r="R5" s="77"/>
+      <c r="S5" s="77"/>
+      <c r="T5" s="77"/>
+      <c r="U5" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="46"/>
-      <c r="W4" s="46"/>
-      <c r="X4" s="46"/>
-      <c r="Y4" s="46"/>
-      <c r="Z4" s="46"/>
-      <c r="AA4" s="46"/>
-      <c r="AB4" s="46" t="s">
+      <c r="V5" s="78"/>
+      <c r="W5" s="78"/>
+      <c r="X5" s="78"/>
+      <c r="Y5" s="78"/>
+      <c r="Z5" s="78"/>
+      <c r="AA5" s="78"/>
+      <c r="AB5" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="AC4" s="46"/>
-      <c r="AD4" s="46"/>
-      <c r="AE4" s="46"/>
-    </row>
-    <row r="5" spans="1:31" ht="26" x14ac:dyDescent="0.3">
-      <c r="A5" s="65" t="s">
+      <c r="AC5" s="78"/>
+      <c r="AD5" s="78"/>
+      <c r="AE5" s="78"/>
+    </row>
+    <row r="6" spans="1:31" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="48"/>
-      <c r="V5" s="49"/>
-      <c r="W5" s="49"/>
-      <c r="X5" s="49"/>
-      <c r="Y5" s="49"/>
-      <c r="Z5" s="49"/>
-      <c r="AA5" s="53"/>
-      <c r="AB5" s="48"/>
-      <c r="AC5" s="49"/>
-      <c r="AD5" s="49"/>
-      <c r="AE5" s="53"/>
-    </row>
-    <row r="6" spans="1:31" ht="26" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="50"/>
-      <c r="V6" s="47"/>
-      <c r="W6" s="47"/>
-      <c r="X6" s="47"/>
-      <c r="Y6" s="47"/>
-      <c r="Z6" s="47"/>
-      <c r="AA6" s="54"/>
-      <c r="AB6" s="50"/>
-      <c r="AC6" s="47"/>
-      <c r="AD6" s="47"/>
-      <c r="AE6" s="54"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="48"/>
+      <c r="V6" s="49"/>
+      <c r="W6" s="49"/>
+      <c r="X6" s="49"/>
+      <c r="Y6" s="49"/>
+      <c r="Z6" s="49"/>
+      <c r="AA6" s="53"/>
+      <c r="AB6" s="48"/>
+      <c r="AC6" s="49"/>
+      <c r="AD6" s="49"/>
+      <c r="AE6" s="53"/>
     </row>
     <row r="7" spans="1:31" ht="26" x14ac:dyDescent="0.3">
       <c r="A7" s="27"/>
@@ -3706,38 +3887,71 @@
       <c r="AD26" s="47"/>
       <c r="AE26" s="54"/>
     </row>
-    <row r="27" spans="1:31" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="28"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="22"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="23"/>
-      <c r="U27" s="51"/>
-      <c r="V27" s="52"/>
-      <c r="W27" s="52"/>
-      <c r="X27" s="52"/>
-      <c r="Y27" s="52"/>
-      <c r="Z27" s="52"/>
-      <c r="AA27" s="55"/>
-      <c r="AB27" s="51"/>
-      <c r="AC27" s="52"/>
-      <c r="AD27" s="52"/>
-      <c r="AE27" s="55"/>
+    <row r="27" spans="1:31" ht="26" x14ac:dyDescent="0.3">
+      <c r="A27" s="27"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="18"/>
+      <c r="U27" s="50"/>
+      <c r="V27" s="47"/>
+      <c r="W27" s="47"/>
+      <c r="X27" s="47"/>
+      <c r="Y27" s="47"/>
+      <c r="Z27" s="47"/>
+      <c r="AA27" s="54"/>
+      <c r="AB27" s="50"/>
+      <c r="AC27" s="47"/>
+      <c r="AD27" s="47"/>
+      <c r="AE27" s="54"/>
+    </row>
+    <row r="28" spans="1:31" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="51"/>
+      <c r="V28" s="52"/>
+      <c r="W28" s="52"/>
+      <c r="X28" s="52"/>
+      <c r="Y28" s="52"/>
+      <c r="Z28" s="52"/>
+      <c r="AA28" s="55"/>
+      <c r="AB28" s="51"/>
+      <c r="AC28" s="52"/>
+      <c r="AD28" s="52"/>
+      <c r="AE28" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3746,10 +3960,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01AD8702-6758-8743-817D-BB1425B49850}">
-  <dimension ref="A1:AF27"/>
+  <dimension ref="A1:AF28"/>
   <sheetViews>
     <sheetView zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6:AF6"/>
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3839,7 +4053,7 @@
       <c r="AE2" s="43"/>
       <c r="AF2" s="56"/>
     </row>
-    <row r="3" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>14</v>
       </c>
@@ -3938,123 +4152,185 @@
       </c>
     </row>
     <row r="4" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="79">
+        <v>1</v>
+      </c>
+      <c r="C4" s="79">
+        <v>2</v>
+      </c>
+      <c r="D4" s="79">
+        <v>3</v>
+      </c>
+      <c r="E4" s="79">
+        <v>4</v>
+      </c>
+      <c r="F4" s="79">
+        <v>5</v>
+      </c>
+      <c r="G4" s="79">
+        <v>6</v>
+      </c>
+      <c r="H4" s="79">
+        <v>7</v>
+      </c>
+      <c r="I4" s="79">
+        <v>8</v>
+      </c>
+      <c r="J4" s="79">
+        <v>9</v>
+      </c>
+      <c r="K4" s="79">
+        <v>10</v>
+      </c>
+      <c r="L4" s="79">
+        <v>11</v>
+      </c>
+      <c r="M4" s="79">
+        <v>12</v>
+      </c>
+      <c r="N4" s="79">
+        <v>13</v>
+      </c>
+      <c r="O4" s="79">
+        <v>14</v>
+      </c>
+      <c r="P4" s="79">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="79">
+        <v>16</v>
+      </c>
+      <c r="R4" s="79">
+        <v>17</v>
+      </c>
+      <c r="S4" s="79">
+        <v>18</v>
+      </c>
+      <c r="T4" s="79">
+        <v>19</v>
+      </c>
+      <c r="U4" s="79">
+        <v>20</v>
+      </c>
+      <c r="V4" s="79">
+        <v>21</v>
+      </c>
+      <c r="W4" s="79">
+        <v>22</v>
+      </c>
+      <c r="X4" s="79">
+        <v>23</v>
+      </c>
+      <c r="Y4" s="79">
+        <v>24</v>
+      </c>
+      <c r="Z4" s="79">
+        <v>25</v>
+      </c>
+      <c r="AA4" s="79">
+        <v>26</v>
+      </c>
+      <c r="AB4" s="79">
+        <v>27</v>
+      </c>
+      <c r="AC4" s="79">
+        <v>28</v>
+      </c>
+      <c r="AD4" s="79">
+        <v>29</v>
+      </c>
+      <c r="AE4" s="79">
+        <v>30</v>
+      </c>
+      <c r="AF4" s="79">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12" t="s">
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12" t="s">
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="77"/>
+      <c r="L5" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="46" t="s">
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="77"/>
+      <c r="R5" s="77"/>
+      <c r="S5" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46"/>
-      <c r="V4" s="46"/>
-      <c r="W4" s="46"/>
-      <c r="X4" s="46"/>
-      <c r="Y4" s="46"/>
-      <c r="Z4" s="46" t="s">
+      <c r="T5" s="78"/>
+      <c r="U5" s="78"/>
+      <c r="V5" s="78"/>
+      <c r="W5" s="78"/>
+      <c r="X5" s="78"/>
+      <c r="Y5" s="78"/>
+      <c r="Z5" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="AA4" s="46"/>
-      <c r="AB4" s="46"/>
-      <c r="AC4" s="46"/>
-      <c r="AD4" s="46"/>
-      <c r="AE4" s="46"/>
-      <c r="AF4" s="46"/>
-    </row>
-    <row r="5" spans="1:32" ht="26" x14ac:dyDescent="0.3">
-      <c r="A5" s="69" t="s">
+      <c r="AA5" s="78"/>
+      <c r="AB5" s="78"/>
+      <c r="AC5" s="78"/>
+      <c r="AD5" s="78"/>
+      <c r="AE5" s="78"/>
+      <c r="AF5" s="78"/>
+    </row>
+    <row r="6" spans="1:32" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="48"/>
-      <c r="T5" s="49"/>
-      <c r="U5" s="49"/>
-      <c r="V5" s="49"/>
-      <c r="W5" s="49"/>
-      <c r="X5" s="59"/>
-      <c r="Y5" s="58"/>
-      <c r="Z5" s="59"/>
-      <c r="AA5" s="59"/>
-      <c r="AB5" s="59"/>
-      <c r="AC5" s="59"/>
-      <c r="AD5" s="59"/>
-      <c r="AE5" s="59"/>
-      <c r="AF5" s="58"/>
-    </row>
-    <row r="6" spans="1:32" ht="26" x14ac:dyDescent="0.3">
-      <c r="A6" s="70" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
+      <c r="W6" s="49"/>
+      <c r="X6" s="59"/>
+      <c r="Y6" s="58"/>
+      <c r="Z6" s="59"/>
+      <c r="AA6" s="59"/>
+      <c r="AB6" s="59"/>
+      <c r="AC6" s="59"/>
+      <c r="AD6" s="59"/>
+      <c r="AE6" s="59"/>
+      <c r="AF6" s="58"/>
+    </row>
+    <row r="7" spans="1:32" ht="26" x14ac:dyDescent="0.3">
+      <c r="A7" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="50"/>
-      <c r="T6" s="47"/>
-      <c r="U6" s="47"/>
-      <c r="V6" s="47"/>
-      <c r="W6" s="47"/>
-      <c r="X6" s="71"/>
-      <c r="Y6" s="71"/>
-      <c r="Z6" s="71"/>
-      <c r="AA6" s="71"/>
-      <c r="AB6" s="71"/>
-      <c r="AC6" s="71"/>
-      <c r="AD6" s="71"/>
-      <c r="AE6" s="71"/>
-      <c r="AF6" s="71"/>
-    </row>
-    <row r="7" spans="1:32" ht="26" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="18"/>
@@ -4077,15 +4353,15 @@
       <c r="U7" s="47"/>
       <c r="V7" s="47"/>
       <c r="W7" s="47"/>
-      <c r="X7" s="47"/>
-      <c r="Y7" s="54"/>
-      <c r="Z7" s="47"/>
-      <c r="AA7" s="47"/>
-      <c r="AB7" s="47"/>
-      <c r="AC7" s="47"/>
-      <c r="AD7" s="47"/>
-      <c r="AE7" s="47"/>
-      <c r="AF7" s="54"/>
+      <c r="X7" s="71"/>
+      <c r="Y7" s="80"/>
+      <c r="Z7" s="71"/>
+      <c r="AA7" s="71"/>
+      <c r="AB7" s="71"/>
+      <c r="AC7" s="71"/>
+      <c r="AD7" s="71"/>
+      <c r="AE7" s="71"/>
+      <c r="AF7" s="71"/>
     </row>
     <row r="8" spans="1:32" ht="26" x14ac:dyDescent="0.3">
       <c r="A8" s="27"/>
@@ -4733,39 +5009,73 @@
       <c r="AE26" s="47"/>
       <c r="AF26" s="54"/>
     </row>
-    <row r="27" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="28"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="23"/>
-      <c r="S27" s="51"/>
-      <c r="T27" s="52"/>
-      <c r="U27" s="52"/>
-      <c r="V27" s="52"/>
-      <c r="W27" s="52"/>
-      <c r="X27" s="52"/>
-      <c r="Y27" s="55"/>
-      <c r="Z27" s="52"/>
-      <c r="AA27" s="52"/>
-      <c r="AB27" s="52"/>
-      <c r="AC27" s="52"/>
-      <c r="AD27" s="52"/>
-      <c r="AE27" s="52"/>
-      <c r="AF27" s="55"/>
+    <row r="27" spans="1:32" ht="26" x14ac:dyDescent="0.3">
+      <c r="A27" s="27"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="50"/>
+      <c r="T27" s="47"/>
+      <c r="U27" s="47"/>
+      <c r="V27" s="47"/>
+      <c r="W27" s="47"/>
+      <c r="X27" s="47"/>
+      <c r="Y27" s="54"/>
+      <c r="Z27" s="47"/>
+      <c r="AA27" s="47"/>
+      <c r="AB27" s="47"/>
+      <c r="AC27" s="47"/>
+      <c r="AD27" s="47"/>
+      <c r="AE27" s="47"/>
+      <c r="AF27" s="54"/>
+    </row>
+    <row r="28" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="51"/>
+      <c r="T28" s="52"/>
+      <c r="U28" s="52"/>
+      <c r="V28" s="52"/>
+      <c r="W28" s="52"/>
+      <c r="X28" s="52"/>
+      <c r="Y28" s="55"/>
+      <c r="Z28" s="52"/>
+      <c r="AA28" s="52"/>
+      <c r="AB28" s="52"/>
+      <c r="AC28" s="52"/>
+      <c r="AD28" s="52"/>
+      <c r="AE28" s="52"/>
+      <c r="AF28" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4774,10 +5084,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A87B0E83-DA68-B340-96CA-9E765341AD44}">
-  <dimension ref="A1:AF26"/>
+  <dimension ref="A1:AF27"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4831,7 +5141,7 @@
       <c r="AE1" s="43"/>
       <c r="AF1" s="43"/>
     </row>
-    <row r="2" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" ht="26" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -4929,133 +5239,195 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:32" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="79"/>
+      <c r="B3" s="79">
+        <v>1</v>
+      </c>
+      <c r="C3" s="79">
+        <v>2</v>
+      </c>
+      <c r="D3" s="79">
+        <v>3</v>
+      </c>
+      <c r="E3" s="79">
+        <v>4</v>
+      </c>
+      <c r="F3" s="79">
+        <v>5</v>
+      </c>
+      <c r="G3" s="79">
+        <v>6</v>
+      </c>
+      <c r="H3" s="79">
+        <v>7</v>
+      </c>
+      <c r="I3" s="79">
+        <v>8</v>
+      </c>
+      <c r="J3" s="79">
+        <v>9</v>
+      </c>
+      <c r="K3" s="79">
+        <v>10</v>
+      </c>
+      <c r="L3" s="79">
+        <v>11</v>
+      </c>
+      <c r="M3" s="79">
+        <v>12</v>
+      </c>
+      <c r="N3" s="79">
+        <v>13</v>
+      </c>
+      <c r="O3" s="79">
+        <v>14</v>
+      </c>
+      <c r="P3" s="79">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="79">
+        <v>16</v>
+      </c>
+      <c r="R3" s="79">
+        <v>17</v>
+      </c>
+      <c r="S3" s="79">
+        <v>18</v>
+      </c>
+      <c r="T3" s="79">
+        <v>19</v>
+      </c>
+      <c r="U3" s="79">
+        <v>20</v>
+      </c>
+      <c r="V3" s="79">
+        <v>21</v>
+      </c>
+      <c r="W3" s="79">
+        <v>22</v>
+      </c>
+      <c r="X3" s="79">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="79">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="79">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="79">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="79">
+        <v>27</v>
+      </c>
+      <c r="AC3" s="79">
+        <v>28</v>
+      </c>
+      <c r="AD3" s="79">
+        <v>29</v>
+      </c>
+      <c r="AE3" s="79">
+        <v>30</v>
+      </c>
+      <c r="AF3" s="79">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12" t="s">
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12" t="s">
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="46" t="s">
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="77"/>
+      <c r="U4" s="77"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="46"/>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="46"/>
-      <c r="AA3" s="46"/>
-      <c r="AB3" s="46"/>
-      <c r="AC3" s="46"/>
-      <c r="AD3" s="46" t="s">
+      <c r="X4" s="78"/>
+      <c r="Y4" s="78"/>
+      <c r="Z4" s="78"/>
+      <c r="AA4" s="78"/>
+      <c r="AB4" s="78"/>
+      <c r="AC4" s="78"/>
+      <c r="AD4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="AE3" s="46"/>
-      <c r="AF3" s="46"/>
-    </row>
-    <row r="4" spans="1:32" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
+      <c r="AE4" s="78"/>
+      <c r="AF4" s="78"/>
+    </row>
+    <row r="5" spans="1:32" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="48"/>
-      <c r="X4" s="49"/>
-      <c r="Y4" s="49"/>
-      <c r="Z4" s="49"/>
-      <c r="AA4" s="49"/>
-      <c r="AB4" s="49"/>
-      <c r="AC4" s="53"/>
-      <c r="AD4" s="48"/>
-      <c r="AE4" s="49"/>
-      <c r="AF4" s="53"/>
-    </row>
-    <row r="5" spans="1:32" ht="26" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="30"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="49"/>
+      <c r="Y5" s="49"/>
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="49"/>
+      <c r="AB5" s="49"/>
+      <c r="AC5" s="53"/>
+      <c r="AD5" s="48"/>
+      <c r="AE5" s="49"/>
+      <c r="AF5" s="53"/>
+    </row>
+    <row r="6" spans="1:32" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="47"/>
-      <c r="Y5" s="47"/>
-      <c r="Z5" s="47"/>
-      <c r="AA5" s="47"/>
-      <c r="AB5" s="47"/>
-      <c r="AC5" s="54"/>
-      <c r="AD5" s="50"/>
-      <c r="AE5" s="47"/>
-      <c r="AF5" s="54"/>
-    </row>
-    <row r="6" spans="1:32" ht="26" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="18"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
       <c r="I6" s="20"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -5727,39 +6099,73 @@
       <c r="AE25" s="47"/>
       <c r="AF25" s="54"/>
     </row>
-    <row r="26" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-      <c r="T26" s="22"/>
-      <c r="U26" s="22"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="51"/>
-      <c r="X26" s="52"/>
-      <c r="Y26" s="52"/>
-      <c r="Z26" s="52"/>
-      <c r="AA26" s="52"/>
-      <c r="AB26" s="52"/>
-      <c r="AC26" s="55"/>
-      <c r="AD26" s="51"/>
-      <c r="AE26" s="52"/>
-      <c r="AF26" s="55"/>
+    <row r="26" spans="1:32" ht="26" x14ac:dyDescent="0.3">
+      <c r="A26" s="27"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="18"/>
+      <c r="W26" s="50"/>
+      <c r="X26" s="47"/>
+      <c r="Y26" s="47"/>
+      <c r="Z26" s="47"/>
+      <c r="AA26" s="47"/>
+      <c r="AB26" s="47"/>
+      <c r="AC26" s="54"/>
+      <c r="AD26" s="50"/>
+      <c r="AE26" s="47"/>
+      <c r="AF26" s="54"/>
+    </row>
+    <row r="27" spans="1:32" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="22"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="51"/>
+      <c r="X27" s="52"/>
+      <c r="Y27" s="52"/>
+      <c r="Z27" s="52"/>
+      <c r="AA27" s="52"/>
+      <c r="AB27" s="52"/>
+      <c r="AC27" s="55"/>
+      <c r="AD27" s="51"/>
+      <c r="AE27" s="52"/>
+      <c r="AF27" s="55"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -5769,15 +6175,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38585A72-1929-CD41-B129-604E7CB15621}">
-  <dimension ref="A1:AD26"/>
+  <dimension ref="A1:AD27"/>
   <sheetViews>
-    <sheetView zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="41" max="41" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5823,7 +6229,7 @@
       <c r="AC1" s="72"/>
       <c r="AD1" s="72"/>
     </row>
-    <row r="2" spans="1:30" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" ht="26" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
@@ -5915,111 +6321,171 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:30" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="79">
+        <v>1</v>
+      </c>
+      <c r="C3" s="79">
+        <v>2</v>
+      </c>
+      <c r="D3" s="79">
+        <v>3</v>
+      </c>
+      <c r="E3" s="79">
+        <v>4</v>
+      </c>
+      <c r="F3" s="79">
+        <v>5</v>
+      </c>
+      <c r="G3" s="79">
+        <v>6</v>
+      </c>
+      <c r="H3" s="79">
+        <v>7</v>
+      </c>
+      <c r="I3" s="79">
+        <v>8</v>
+      </c>
+      <c r="J3" s="79">
+        <v>9</v>
+      </c>
+      <c r="K3" s="79">
+        <v>10</v>
+      </c>
+      <c r="L3" s="79">
+        <v>11</v>
+      </c>
+      <c r="M3" s="79">
+        <v>12</v>
+      </c>
+      <c r="N3" s="79">
+        <v>13</v>
+      </c>
+      <c r="O3" s="79">
+        <v>14</v>
+      </c>
+      <c r="P3" s="79">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="79">
+        <v>16</v>
+      </c>
+      <c r="R3" s="79">
+        <v>17</v>
+      </c>
+      <c r="S3" s="79">
+        <v>18</v>
+      </c>
+      <c r="T3" s="79">
+        <v>19</v>
+      </c>
+      <c r="U3" s="79">
+        <v>20</v>
+      </c>
+      <c r="V3" s="79">
+        <v>21</v>
+      </c>
+      <c r="W3" s="79">
+        <v>22</v>
+      </c>
+      <c r="X3" s="79">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="79">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="79">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="79">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="79">
+        <v>27</v>
+      </c>
+      <c r="AC3" s="79">
+        <v>28</v>
+      </c>
+      <c r="AD3" s="79">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12" t="s">
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12" t="s">
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="46" t="s">
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="46"/>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="46"/>
-      <c r="AA3" s="46" t="s">
+      <c r="U4" s="78"/>
+      <c r="V4" s="78"/>
+      <c r="W4" s="78"/>
+      <c r="X4" s="78"/>
+      <c r="Y4" s="78"/>
+      <c r="Z4" s="78"/>
+      <c r="AA4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="AB3" s="46"/>
-      <c r="AC3" s="46"/>
-      <c r="AD3" s="46"/>
-    </row>
-    <row r="4" spans="1:30" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="48"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="49"/>
-      <c r="W4" s="49"/>
-      <c r="X4" s="49"/>
-      <c r="Y4" s="49"/>
-      <c r="Z4" s="53"/>
-      <c r="AA4" s="49"/>
-      <c r="AB4" s="49"/>
-      <c r="AC4" s="49"/>
-      <c r="AD4" s="49"/>
+      <c r="AB4" s="78"/>
+      <c r="AC4" s="78"/>
+      <c r="AD4" s="78"/>
     </row>
     <row r="5" spans="1:30" ht="26" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="47"/>
-      <c r="V5" s="47"/>
-      <c r="W5" s="47"/>
-      <c r="X5" s="47"/>
-      <c r="Y5" s="47"/>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="47"/>
-      <c r="AB5" s="47"/>
-      <c r="AC5" s="47"/>
-      <c r="AD5" s="47"/>
+      <c r="A5" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="49"/>
+      <c r="V5" s="49"/>
+      <c r="W5" s="49"/>
+      <c r="X5" s="49"/>
+      <c r="Y5" s="49"/>
+      <c r="Z5" s="53"/>
+      <c r="AA5" s="49"/>
+      <c r="AB5" s="49"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="49"/>
     </row>
     <row r="6" spans="1:30" ht="26" x14ac:dyDescent="0.3">
       <c r="A6" s="27"/>
@@ -6661,37 +7127,69 @@
       <c r="AC25" s="47"/>
       <c r="AD25" s="47"/>
     </row>
-    <row r="26" spans="1:30" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="51"/>
-      <c r="U26" s="52"/>
-      <c r="V26" s="52"/>
-      <c r="W26" s="52"/>
-      <c r="X26" s="52"/>
-      <c r="Y26" s="52"/>
-      <c r="Z26" s="55"/>
-      <c r="AA26" s="52"/>
-      <c r="AB26" s="52"/>
-      <c r="AC26" s="52"/>
-      <c r="AD26" s="52"/>
+    <row r="26" spans="1:30" ht="26" x14ac:dyDescent="0.3">
+      <c r="A26" s="27"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="47"/>
+      <c r="V26" s="47"/>
+      <c r="W26" s="47"/>
+      <c r="X26" s="47"/>
+      <c r="Y26" s="47"/>
+      <c r="Z26" s="54"/>
+      <c r="AA26" s="47"/>
+      <c r="AB26" s="47"/>
+      <c r="AC26" s="47"/>
+      <c r="AD26" s="47"/>
+    </row>
+    <row r="27" spans="1:30" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="51"/>
+      <c r="U27" s="52"/>
+      <c r="V27" s="52"/>
+      <c r="W27" s="52"/>
+      <c r="X27" s="52"/>
+      <c r="Y27" s="52"/>
+      <c r="Z27" s="55"/>
+      <c r="AA27" s="52"/>
+      <c r="AB27" s="52"/>
+      <c r="AC27" s="52"/>
+      <c r="AD27" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>